<commit_message>
Nem sei mais oq mudou
</commit_message>
<xml_diff>
--- a/Database/WorldsMatches.xlsx
+++ b/Database/WorldsMatches.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Dudu\Documents\Trabalhos do Dudu\Projects\8º Semestre\Aplicação de ML e DM\League-of-Legends-World-s-predictor\Database\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{55255F13-E239-4E80-BF7C-61059D86F0E3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DBB9562D-F805-4994-91D9-947E61905ABC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="113" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="157" uniqueCount="21">
   <si>
     <t>Azul</t>
   </si>
@@ -89,7 +89,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="19" x14ac:knownFonts="1">
+  <fonts count="20" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -231,6 +231,12 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF222222"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="33">
@@ -574,9 +580,13 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Ênfase1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -932,10 +942,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E55"/>
+  <dimension ref="A1:G77"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+    <sheetView tabSelected="1" topLeftCell="A53" workbookViewId="0">
+      <selection activeCell="G77" sqref="G77"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1875,6 +1885,382 @@
         <v>0</v>
       </c>
     </row>
+    <row r="56" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A56" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B56" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C56" s="2">
+        <v>1</v>
+      </c>
+      <c r="D56">
+        <v>1</v>
+      </c>
+      <c r="E56">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="57" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A57" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="B57" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C57" s="2">
+        <v>1</v>
+      </c>
+      <c r="D57">
+        <v>1</v>
+      </c>
+      <c r="E57">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="58" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A58" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B58" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="C58" s="2">
+        <v>1</v>
+      </c>
+      <c r="D58">
+        <v>1</v>
+      </c>
+      <c r="E58">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="59" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A59" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B59" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="C59" s="2">
+        <v>0</v>
+      </c>
+      <c r="D59">
+        <v>1</v>
+      </c>
+      <c r="E59">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="60" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A60" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B60" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="C60" s="2">
+        <v>1</v>
+      </c>
+      <c r="D60">
+        <v>1</v>
+      </c>
+      <c r="E60">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="61" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A61" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="B61" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C61" s="2">
+        <v>1</v>
+      </c>
+      <c r="D61">
+        <v>1</v>
+      </c>
+      <c r="E61">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="62" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A62" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="B62" t="s">
+        <v>18</v>
+      </c>
+      <c r="C62" s="2">
+        <v>1</v>
+      </c>
+      <c r="D62">
+        <v>1</v>
+      </c>
+      <c r="E62">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="63" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A63" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B63" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="C63" s="2">
+        <v>1</v>
+      </c>
+      <c r="D63">
+        <v>1</v>
+      </c>
+      <c r="E63">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="64" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A64" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="B64" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C64" s="2">
+        <v>0</v>
+      </c>
+      <c r="D64">
+        <v>1</v>
+      </c>
+      <c r="E64">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="65" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A65" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="B65" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C65" s="2">
+        <v>0</v>
+      </c>
+      <c r="D65">
+        <v>1</v>
+      </c>
+      <c r="E65">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="66" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A66" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="B66" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C66" s="2">
+        <v>1</v>
+      </c>
+      <c r="D66">
+        <v>1</v>
+      </c>
+      <c r="E66">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="67" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A67" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B67" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="C67" s="2">
+        <v>1</v>
+      </c>
+      <c r="D67">
+        <v>1</v>
+      </c>
+      <c r="E67">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="68" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A68" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="B68" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C68" s="2">
+        <v>0</v>
+      </c>
+      <c r="D68">
+        <v>1</v>
+      </c>
+      <c r="E68">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="69" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A69" t="s">
+        <v>18</v>
+      </c>
+      <c r="B69" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C69" s="2">
+        <v>0</v>
+      </c>
+      <c r="D69">
+        <v>1</v>
+      </c>
+      <c r="E69">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="70" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A70" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B70" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C70" s="2">
+        <v>1</v>
+      </c>
+      <c r="D70">
+        <v>1</v>
+      </c>
+      <c r="E70">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="71" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A71" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="B71" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="C71" s="2">
+        <v>1</v>
+      </c>
+      <c r="D71">
+        <v>1</v>
+      </c>
+      <c r="E71">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="72" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A72" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="B72" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C72" s="2">
+        <v>0</v>
+      </c>
+      <c r="D72">
+        <v>1</v>
+      </c>
+      <c r="E72">
+        <v>0</v>
+      </c>
+      <c r="G72" s="1"/>
+    </row>
+    <row r="73" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A73" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B73" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="C73" s="2">
+        <v>1</v>
+      </c>
+      <c r="D73">
+        <v>1</v>
+      </c>
+      <c r="E73">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="74" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A74" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B74" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C74" s="2">
+        <v>1</v>
+      </c>
+      <c r="D74">
+        <v>1</v>
+      </c>
+      <c r="E74">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="75" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A75" t="s">
+        <v>18</v>
+      </c>
+      <c r="B75" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="C75" s="2">
+        <v>1</v>
+      </c>
+      <c r="D75">
+        <v>1</v>
+      </c>
+      <c r="E75">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="76" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A76" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="B76" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="C76" s="2">
+        <v>0</v>
+      </c>
+      <c r="D76">
+        <v>1</v>
+      </c>
+      <c r="E76">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="77" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A77" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="B77" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C77" s="2">
+        <v>0</v>
+      </c>
+      <c r="D77">
+        <v>1</v>
+      </c>
+      <c r="E77">
+        <v>0</v>
+      </c>
+      <c r="G77" s="3"/>
+    </row>
   </sheetData>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>